<commit_message>
Finalised and tested Session and Transaction classes. Working on SessionUpload class.
</commit_message>
<xml_diff>
--- a/Library/Templates/CWR_Checklist_Template.xlsx
+++ b/Library/Templates/CWR_Checklist_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33220" yWindow="780" windowWidth="25540" windowHeight="17300" tabRatio="724"/>
+    <workbookView xWindow="-33220" yWindow="780" windowWidth="25540" windowHeight="17300" tabRatio="724" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Read this" sheetId="13" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="394">
   <si>
     <t xml:space="preserve">Country code identifying the National CWR checklist; the code of the country preparing the CWR checklist. For country codes use the three-letter ISO 3166-1 (see: http://unstats.un.org/unsd/methods/m49/m49alpha.htm ) </t>
   </si>
@@ -2152,15 +2152,12 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
-  <si>
-    <t>template::checklist:cwr</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2363,6 +2360,13 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2838,7 +2842,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="106">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -2963,15 +2967,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>15874</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>41274</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>625475</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>117475</xdr:rowOff>
+      <xdr:colOff>663575</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2980,8 +2984,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="193674"/>
-          <a:ext cx="9998075" cy="10769601"/>
+          <a:off x="38100" y="41274"/>
+          <a:ext cx="10455275" cy="10769601"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4341,17 +4345,17 @@
   <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="72" t="s">
-        <v>394</v>
-      </c>
+    <row r="1" spans="1:1" ht="23">
+      <c r="A1" s="72"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4370,9 +4374,9 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5594,7 +5598,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="87" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Changed and added error types and codes. Finalised data copy in SessionUpload, working on object creation. Changed template iterator by making 'K' element worksheet key field name and 'F' element worksheet relation field. Updated ":taxon:reference" tag: changed URL data type to string -> is in update xml 3. Added another test template to have controlled and few results.
</commit_message>
<xml_diff>
--- a/Library/Templates/CWR_Checklist_Template.xlsx
+++ b/Library/Templates/CWR_Checklist_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33220" yWindow="780" windowWidth="25540" windowHeight="17300" tabRatio="724" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="724" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Read this" sheetId="13" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="394">
   <si>
     <t xml:space="preserve">Country code identifying the National CWR checklist; the code of the country preparing the CWR checklist. For country codes use the three-letter ISO 3166-1 (see: http://unstats.un.org/unsd/methods/m49/m49alpha.htm ) </t>
   </si>
@@ -2841,8 +2841,8 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="106">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4355,7 +4355,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="23">
-      <c r="A1" s="72"/>
+      <c r="A1" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4374,7 +4374,7 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
@@ -5247,9 +5247,9 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5452,7 +5452,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="18" customFormat="1" ht="28">
+    <row r="6" spans="1:20" s="18" customFormat="1">
       <c r="A6" s="52"/>
       <c r="B6" s="35" t="s">
         <v>335</v>
@@ -5465,9 +5465,7 @@
         <v>343</v>
       </c>
       <c r="F6" s="35"/>
-      <c r="G6" s="35" t="s">
-        <v>186</v>
-      </c>
+      <c r="G6" s="35"/>
       <c r="H6" s="35" t="s">
         <v>354</v>
       </c>
@@ -5627,7 +5625,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="56">
-      <c r="A2" s="71"/>
+      <c r="A2" s="72"/>
       <c r="B2" s="20" t="s">
         <v>145</v>
       </c>
@@ -5640,7 +5638,7 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="42">
-      <c r="A3" s="71"/>
+      <c r="A3" s="72"/>
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
@@ -5655,7 +5653,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="140">
-      <c r="A4" s="71"/>
+      <c r="A4" s="72"/>
       <c r="B4" s="5" t="s">
         <v>99</v>
       </c>
@@ -5670,7 +5668,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="70">
-      <c r="A5" s="71"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="5" t="s">
         <v>100</v>
       </c>
@@ -5685,7 +5683,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="98">
-      <c r="A6" s="71"/>
+      <c r="A6" s="72"/>
       <c r="B6" s="5" t="s">
         <v>101</v>
       </c>
@@ -5698,7 +5696,7 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" ht="42">
-      <c r="A7" s="71"/>
+      <c r="A7" s="72"/>
       <c r="B7" s="5" t="s">
         <v>102</v>
       </c>
@@ -5711,7 +5709,7 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="28">
-      <c r="A8" s="71"/>
+      <c r="A8" s="72"/>
       <c r="B8" s="5" t="s">
         <v>142</v>
       </c>
@@ -5724,7 +5722,7 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="56">
-      <c r="A9" s="71"/>
+      <c r="A9" s="72"/>
       <c r="B9" s="16" t="s">
         <v>103</v>
       </c>
@@ -5737,7 +5735,7 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="71"/>
+      <c r="A10" s="72"/>
       <c r="B10" s="5" t="s">
         <v>98</v>
       </c>
@@ -5750,7 +5748,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="28">
-      <c r="A11" s="71"/>
+      <c r="A11" s="72"/>
       <c r="B11" s="5" t="s">
         <v>104</v>
       </c>
@@ -5763,7 +5761,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="28">
-      <c r="A12" s="71"/>
+      <c r="A12" s="72"/>
       <c r="B12" s="5" t="s">
         <v>105</v>
       </c>
@@ -5776,7 +5774,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="28">
-      <c r="A13" s="71"/>
+      <c r="A13" s="72"/>
       <c r="B13" s="5" t="s">
         <v>106</v>
       </c>
@@ -5789,7 +5787,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="28">
-      <c r="A14" s="71"/>
+      <c r="A14" s="72"/>
       <c r="B14" s="5" t="s">
         <v>107</v>
       </c>
@@ -5802,7 +5800,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="71"/>
+      <c r="A15" s="72"/>
       <c r="B15" s="5" t="s">
         <v>108</v>
       </c>
@@ -5817,7 +5815,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="28">
-      <c r="A16" s="71"/>
+      <c r="A16" s="72"/>
       <c r="B16" s="5" t="s">
         <v>109</v>
       </c>
@@ -5832,7 +5830,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="71"/>
+      <c r="A17" s="72"/>
       <c r="B17" s="5" t="s">
         <v>110</v>
       </c>
@@ -5847,7 +5845,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="56">
-      <c r="A18" s="71"/>
+      <c r="A18" s="72"/>
       <c r="B18" s="5" t="s">
         <v>111</v>
       </c>
@@ -5862,7 +5860,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="71"/>
+      <c r="A19" s="72"/>
       <c r="B19" s="5" t="s">
         <v>112</v>
       </c>
@@ -5877,7 +5875,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="28">
-      <c r="A20" s="71"/>
+      <c r="A20" s="72"/>
       <c r="B20" s="5" t="s">
         <v>113</v>
       </c>
@@ -5892,7 +5890,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="70">
-      <c r="A21" s="71"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="5" t="s">
         <v>114</v>
       </c>
@@ -5905,7 +5903,7 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="42">
-      <c r="A22" s="71"/>
+      <c r="A22" s="72"/>
       <c r="B22" s="5" t="s">
         <v>115</v>
       </c>
@@ -5920,7 +5918,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="28">
-      <c r="A23" s="71"/>
+      <c r="A23" s="72"/>
       <c r="B23" s="5" t="s">
         <v>116</v>
       </c>
@@ -5933,7 +5931,7 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="120" customHeight="1">
-      <c r="A24" s="71"/>
+      <c r="A24" s="72"/>
       <c r="B24" s="22" t="s">
         <v>151</v>
       </c>
@@ -5950,7 +5948,7 @@
       <c r="G24" s="25"/>
     </row>
     <row r="25" spans="1:7" ht="36">
-      <c r="A25" s="71"/>
+      <c r="A25" s="72"/>
       <c r="B25" s="5" t="s">
         <v>117</v>
       </c>
@@ -5967,7 +5965,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="60">
-      <c r="A26" s="71"/>
+      <c r="A26" s="72"/>
       <c r="B26" s="5" t="s">
         <v>118</v>
       </c>
@@ -5982,7 +5980,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="28">
-      <c r="A27" s="71"/>
+      <c r="A27" s="72"/>
       <c r="B27" s="5" t="s">
         <v>119</v>
       </c>
@@ -5995,7 +5993,7 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="56">
-      <c r="A28" s="71"/>
+      <c r="A28" s="72"/>
       <c r="B28" s="5" t="s">
         <v>120</v>
       </c>
@@ -6008,7 +6006,7 @@
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:7" ht="28">
-      <c r="A29" s="71"/>
+      <c r="A29" s="72"/>
       <c r="B29" s="5" t="s">
         <v>122</v>
       </c>
@@ -6021,7 +6019,7 @@
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:7" ht="112">
-      <c r="A30" s="71"/>
+      <c r="A30" s="72"/>
       <c r="B30" s="5" t="s">
         <v>121</v>
       </c>
@@ -6034,7 +6032,7 @@
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:7" ht="28">
-      <c r="A31" s="71"/>
+      <c r="A31" s="72"/>
       <c r="B31" s="5" t="s">
         <v>123</v>
       </c>
@@ -6060,7 +6058,7 @@
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" ht="56">
-      <c r="A33" s="71"/>
+      <c r="A33" s="72"/>
       <c r="B33" s="20" t="s">
         <v>145</v>
       </c>
@@ -6073,7 +6071,7 @@
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" ht="28">
-      <c r="A34" s="71"/>
+      <c r="A34" s="72"/>
       <c r="B34" s="5" t="s">
         <v>125</v>
       </c>
@@ -6086,7 +6084,7 @@
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="28">
-      <c r="A35" s="71"/>
+      <c r="A35" s="72"/>
       <c r="B35" s="5" t="s">
         <v>127</v>
       </c>
@@ -6099,7 +6097,7 @@
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" ht="56">
-      <c r="A36" s="71"/>
+      <c r="A36" s="72"/>
       <c r="B36" s="5" t="s">
         <v>126</v>
       </c>
@@ -6112,7 +6110,7 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" ht="28">
-      <c r="A37" s="71"/>
+      <c r="A37" s="72"/>
       <c r="B37" s="5" t="s">
         <v>128</v>
       </c>
@@ -6138,7 +6136,7 @@
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" ht="56">
-      <c r="A39" s="71"/>
+      <c r="A39" s="72"/>
       <c r="B39" s="20" t="s">
         <v>145</v>
       </c>
@@ -6151,7 +6149,7 @@
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="71"/>
+      <c r="A40" s="72"/>
       <c r="B40" s="5" t="s">
         <v>130</v>
       </c>
@@ -6166,7 +6164,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="42">
-      <c r="A41" s="71"/>
+      <c r="A41" s="72"/>
       <c r="B41" s="5" t="s">
         <v>131</v>
       </c>
@@ -6179,7 +6177,7 @@
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" ht="84">
-      <c r="A42" s="71"/>
+      <c r="A42" s="72"/>
       <c r="B42" s="5" t="s">
         <v>132</v>
       </c>
@@ -6192,7 +6190,7 @@
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" ht="56">
-      <c r="A43" s="71"/>
+      <c r="A43" s="72"/>
       <c r="B43" s="5" t="s">
         <v>133</v>
       </c>
@@ -6205,7 +6203,7 @@
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" ht="56">
-      <c r="A44" s="71"/>
+      <c r="A44" s="72"/>
       <c r="B44" s="5" t="s">
         <v>134</v>
       </c>
@@ -6218,7 +6216,7 @@
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" ht="56">
-      <c r="A45" s="71"/>
+      <c r="A45" s="72"/>
       <c r="B45" s="5" t="s">
         <v>134</v>
       </c>
@@ -6231,7 +6229,7 @@
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="29">
-      <c r="A46" s="71"/>
+      <c r="A46" s="72"/>
       <c r="B46" s="5" t="s">
         <v>135</v>
       </c>
@@ -6244,7 +6242,7 @@
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" ht="42">
-      <c r="A47" s="71"/>
+      <c r="A47" s="72"/>
       <c r="B47" s="5" t="s">
         <v>136</v>
       </c>
@@ -6257,7 +6255,7 @@
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" ht="406">
-      <c r="A48" s="71"/>
+      <c r="A48" s="72"/>
       <c r="B48" s="5" t="s">
         <v>137</v>
       </c>
@@ -6270,7 +6268,7 @@
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="1:5" ht="266">
-      <c r="A49" s="71"/>
+      <c r="A49" s="72"/>
       <c r="B49" s="5" t="s">
         <v>138</v>
       </c>
@@ -6283,7 +6281,7 @@
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" ht="70">
-      <c r="A50" s="71"/>
+      <c r="A50" s="72"/>
       <c r="B50" s="5" t="s">
         <v>139</v>
       </c>
@@ -6296,7 +6294,7 @@
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" ht="42">
-      <c r="A51" s="71" t="s">
+      <c r="A51" s="72" t="s">
         <v>155</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -6311,7 +6309,7 @@
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" ht="70">
-      <c r="A52" s="71"/>
+      <c r="A52" s="72"/>
       <c r="B52" s="5" t="s">
         <v>141</v>
       </c>
@@ -6324,7 +6322,7 @@
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" ht="56">
-      <c r="A53" s="71"/>
+      <c r="A53" s="72"/>
       <c r="B53" s="5"/>
       <c r="C53" s="3" t="s">
         <v>168</v>

</xml_diff>

<commit_message>
Added rejected value to validated flag: so we also have errors. Added kTAG_ROW to save row number in objects in order to signal duplicate object row. Changed log entries in init scripts. Added collection to transformation elements in template standards: forgot them, UPDATES_META.04.xml holds the added collections.
</commit_message>
<xml_diff>
--- a/Library/Templates/CWR_Checklist_Template.xlsx
+++ b/Library/Templates/CWR_Checklist_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="724" activeTab="3"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="724" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Read this" sheetId="13" r:id="rId1"/>
@@ -1865,9 +1865,6 @@
     <t>SUCCROSSREF</t>
   </si>
   <si>
-    <t>Indicate the percentage (%) of success rate for each cross. Multiple values are separated by semicolon (;) without space.</t>
-  </si>
-  <si>
     <t>Population type</t>
   </si>
   <si>
@@ -2151,6 +2148,9 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t>Indicate the percentage (%) of success rate for each cross.</t>
   </si>
 </sst>
 </file>
@@ -4374,9 +4374,9 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5127,7 +5127,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18">
       <c r="A1" s="44" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -5137,7 +5137,7 @@
     </row>
     <row r="2" spans="1:6" ht="15">
       <c r="A2" s="47" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -5170,7 +5170,7 @@
         <v>321</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="70">
@@ -5187,10 +5187,10 @@
         <v>320</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>323</v>
+        <v>393</v>
       </c>
       <c r="F5" s="61" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5228,7 +5228,7 @@
         <v>322</v>
       </c>
       <c r="F8" s="63" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -5247,9 +5247,9 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5260,7 +5260,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="18">
       <c r="A1" s="44" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -5284,7 +5284,7 @@
     </row>
     <row r="2" spans="1:20" s="18" customFormat="1" ht="15">
       <c r="A2" s="47" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -5333,150 +5333,150 @@
         <v>170</v>
       </c>
       <c r="B4" s="64" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C4" s="64" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D4" s="64" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G4" s="64" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H4" s="64" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I4" s="64" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J4" s="64" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K4" s="64" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L4" s="64" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M4" s="66" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="N4" s="66" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="O4" s="64" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="P4" s="64" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="Q4" s="64" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="R4" s="64" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="S4" s="64" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="T4" s="69" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="18" customFormat="1" ht="224">
       <c r="A5" s="50" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C5" s="41" t="s">
         <v>45</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G5" s="41" t="s">
         <v>47</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I5" s="41" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J5" s="41" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K5" s="41" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="M5" s="42" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="N5" s="34" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="O5" s="34" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P5" s="34" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="Q5" s="34" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="R5" s="34" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S5" s="34" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="T5" s="51" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="18" customFormat="1">
       <c r="A6" s="52"/>
       <c r="B6" s="35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C6" s="35"/>
       <c r="D6" s="35" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F6" s="35"/>
       <c r="G6" s="35"/>
       <c r="H6" s="35" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J6" s="35"/>
       <c r="K6" s="35"/>
       <c r="L6" s="35"/>
       <c r="M6" s="35" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="N6" s="35"/>
       <c r="O6" s="36"/>
@@ -5484,7 +5484,7 @@
       <c r="Q6" s="36"/>
       <c r="R6" s="36"/>
       <c r="S6" s="36" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="T6" s="70"/>
     </row>
@@ -5519,61 +5519,61 @@
         <v>172</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D8" s="57" t="s">
+        <v>346</v>
+      </c>
+      <c r="E8" s="57" t="s">
         <v>347</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="F8" s="57" t="s">
         <v>348</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="G8" s="57" t="s">
         <v>349</v>
       </c>
-      <c r="G8" s="57" t="s">
-        <v>350</v>
-      </c>
       <c r="H8" s="57" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I8" s="57" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J8" s="57" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K8" s="57" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L8" s="57" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M8" s="57" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="N8" s="57" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O8" s="57" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="P8" s="57" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="Q8" s="57" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="R8" s="58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="S8" s="58" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="T8" s="59" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>